<commit_message>
Push organization of files
Push organization of files
</commit_message>
<xml_diff>
--- a/results_excel.xlsx
+++ b/results_excel.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\GitHub\DE_Basin_CWSRF_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34D58F21-6DE2-4ED5-A185-7B78BDAF0C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6617915-2966-4A6C-B424-EEA2F9A4FAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{3D4A5D89-EFAC-4575-BF68-0B5671E3F749}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{3D4A5D89-EFAC-4575-BF68-0B5671E3F749}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$H$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$J$25</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Wayne</t>
   </si>
   <si>
-    <t>PA</t>
-  </si>
-  <si>
     <t>Philadelphia</t>
   </si>
   <si>
@@ -70,18 +67,12 @@
     <t>New Castle</t>
   </si>
   <si>
-    <t>DE</t>
-  </si>
-  <si>
     <t>Kent</t>
   </si>
   <si>
     <t>Sussex</t>
   </si>
   <si>
-    <t>NJ</t>
-  </si>
-  <si>
     <t>Camden</t>
   </si>
   <si>
@@ -128,15 +119,29 @@
   </si>
   <si>
     <t>Percent of Urban Population that is also overburdend</t>
+  </si>
+  <si>
+    <t>CWSRF Subsidy, July 2018 to June 2023</t>
+  </si>
+  <si>
+    <t>Subsidy per Urban Capita ($)</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -597,7 +602,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -642,6 +647,7 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -651,23 +657,25 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="25" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="29" builtinId="38" customBuiltin="1"/>
@@ -695,6 +703,7 @@
     <cellStyle name="Bad" xfId="9" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="13" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="15" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Explanatory Text" xfId="18" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="8" builtinId="26" customBuiltin="1"/>
@@ -1043,675 +1052,828 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368E7D20-9635-4E47-860B-FD9183803BB6}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="A1:H25"/>
+      <selection activeCell="J25" sqref="A1:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="36.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7">
+        <v>990099</v>
+      </c>
+      <c r="D2" s="7">
+        <v>495050</v>
+      </c>
+      <c r="E2" s="9">
+        <v>116374</v>
+      </c>
+      <c r="F2" s="7">
+        <v>8.5079055459123207</v>
+      </c>
+      <c r="G2" s="7">
+        <v>4.2539570694485001</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0.75490000000000002</v>
+      </c>
+      <c r="I2" s="8">
+        <v>9.5399999999999999E-2</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.662759722962174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C3" s="7">
+        <v>128491720</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1603797</v>
+      </c>
+      <c r="F3" s="7">
+        <v>80.117196877160893</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="8">
+      <c r="I3" s="8">
+        <v>0.99570000000000003</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.63713674486234895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="7">
         <v>8962296.6799999997</v>
       </c>
-      <c r="D2" s="3">
-        <v>2900</v>
-      </c>
-      <c r="E2" s="8">
-        <v>3090.4471310344802</v>
-      </c>
-      <c r="F2" s="4">
-        <v>5.67E-2</v>
-      </c>
-      <c r="G2" s="4">
-        <v>9.1999999999999998E-3</v>
-      </c>
-      <c r="H2" s="4">
-        <v>0.74896551724137894</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="D4" s="7">
+        <v>1835424</v>
+      </c>
+      <c r="E4" s="9">
+        <v>7018</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1277.04426902251</v>
+      </c>
+      <c r="G4" s="7">
+        <v>261.530920490168</v>
+      </c>
+      <c r="H4" s="8">
+        <v>0.13719999999999999</v>
+      </c>
+      <c r="I4" s="8">
+        <v>7.6E-3</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.59874608150470199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>75653</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.52890000000000004</v>
+      </c>
+      <c r="I5" s="8">
+        <v>3.9100000000000003E-2</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.43174758436545801</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>26601</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.4108</v>
+      </c>
+      <c r="I6" s="8">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.34840795458817297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="7">
+        <v>35389161</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2100000</v>
+      </c>
+      <c r="E7" s="9">
+        <v>367671</v>
+      </c>
+      <c r="F7" s="7">
+        <v>96.252249973481696</v>
+      </c>
+      <c r="G7" s="7">
+        <v>5.7116280587808097</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.94920000000000004</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.55559999999999998</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.34704396049729203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3428796</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>30371</v>
+      </c>
+      <c r="F8" s="7">
+        <v>112.897039939416</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.46839999999999998</v>
+      </c>
+      <c r="I8" s="8">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.33235652431595902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="7">
+        <v>832739</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>314967</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2.6438928522670602</v>
+      </c>
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0.73440000000000005</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.13880000000000001</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.30124108239910802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>337572</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.90129999999999999</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.39710000000000001</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.28895761496806599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="7">
+        <v>168732364</v>
+      </c>
+      <c r="D11" s="7">
+        <v>25674445</v>
+      </c>
+      <c r="E11" s="9">
+        <v>516639</v>
+      </c>
+      <c r="F11" s="7">
+        <v>326.59625773509202</v>
+      </c>
+      <c r="G11" s="7">
+        <v>49.695135287889599</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.9869</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.70630000000000004</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.24572283548086801</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7">
+        <v>28479181</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>133471</v>
+      </c>
+      <c r="F12" s="7">
+        <v>213.37354931033701</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.23587895497898401</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>7366</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.1258</v>
+      </c>
+      <c r="I13" s="8">
+        <v>2.6700000000000002E-2</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.208254140646212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7">
+        <v>42819075.789999999</v>
+      </c>
+      <c r="D14" s="7">
+        <v>7006039</v>
+      </c>
+      <c r="E14" s="9">
+        <v>572034</v>
+      </c>
+      <c r="F14" s="7">
+        <v>74.854074740312598</v>
+      </c>
+      <c r="G14" s="7">
+        <v>12.247591926354</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.99170000000000003</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.86080000000000001</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.17214011754546099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2490000</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>259980</v>
+      </c>
+      <c r="F15" s="7">
+        <v>9.5776598199861507</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0.83069999999999999</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.31509999999999999</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.17037849065312699</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="7">
+        <v>29893961</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>77106</v>
+      </c>
+      <c r="F16" s="7">
+        <v>387.69954348559099</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.80940000000000001</v>
+      </c>
+      <c r="I16" s="8">
+        <v>9.8699999999999996E-2</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.162594350634192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>72434</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.43030000000000002</v>
+      </c>
+      <c r="I17" s="8">
+        <v>9.6299999999999997E-2</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.155810807079548</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7">
+        <v>80700713</v>
+      </c>
+      <c r="D18" s="7">
+        <v>997000</v>
+      </c>
+      <c r="E18" s="9">
+        <v>535938</v>
+      </c>
+      <c r="F18" s="7">
+        <v>150.57844937287501</v>
+      </c>
+      <c r="G18" s="7">
+        <v>1.8602898096421601</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0.93910000000000005</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.46079999999999999</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.14262097481425101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="7">
+        <v>26230114</v>
+      </c>
+      <c r="D19" s="7">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>62271</v>
+      </c>
+      <c r="F19" s="7">
+        <v>421.22519310754598</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="I19" s="8">
+        <v>6.6900000000000001E-2</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0.129610894316777</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="8">
-        <v>990099</v>
-      </c>
-      <c r="D3" s="3">
-        <v>102786</v>
-      </c>
-      <c r="E3" s="8">
-        <v>9.6326250656704193</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.66679999999999995</v>
-      </c>
-      <c r="G3" s="4">
-        <v>9.74E-2</v>
-      </c>
-      <c r="H3" s="4">
-        <v>0.74747533710816694</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="8">
-        <v>128491720</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1603797</v>
-      </c>
-      <c r="E4" s="8">
-        <v>80.117196877160893</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0.63735747105151097</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="7">
+        <v>43923508</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1783138</v>
+      </c>
+      <c r="E20" s="9">
+        <v>416722</v>
+      </c>
+      <c r="F20" s="7">
+        <v>105.40242175839001</v>
+      </c>
+      <c r="G20" s="7">
+        <v>4.2789629537197502</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.90229999999999999</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.25090000000000001</v>
+      </c>
+      <c r="J20" s="8">
+        <v>6.9710742413407495E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>74571</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.52129999999999999</v>
-      </c>
-      <c r="G5" s="4">
-        <v>5.8599999999999999E-2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>0.42178594896139304</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1349794.92</v>
+      </c>
+      <c r="D21" s="7">
+        <v>4163298.87</v>
+      </c>
+      <c r="E21" s="9">
+        <v>431257</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3.1299084304718501</v>
+      </c>
+      <c r="G21" s="7">
+        <v>9.6538696647242794</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0.37959999999999999</v>
+      </c>
+      <c r="J21" s="8">
+        <v>6.6185592349805297E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>23359</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.36080000000000001</v>
-      </c>
-      <c r="G6" s="4">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0.40194357635172701</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="8">
-        <v>35389161</v>
-      </c>
-      <c r="D7" s="3">
-        <v>353632</v>
-      </c>
-      <c r="E7" s="8">
-        <v>100.07341247398401</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.53439999999999999</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0.359300063342684</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="8">
-        <v>3428796</v>
-      </c>
-      <c r="D8" s="3">
-        <v>29488</v>
-      </c>
-      <c r="E8" s="8">
-        <v>116.277672273467</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.45479999999999998</v>
-      </c>
-      <c r="G8" s="4">
-        <v>4.4400000000000002E-2</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.34363130765056998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="8">
-        <v>832739</v>
-      </c>
-      <c r="D9" s="3">
-        <v>298239</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2.7921868032014601</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.69540000000000002</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.1784</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0.31439214857882403</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>333640</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.89410000000000001</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0.48609999999999998</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0.29253386884066701</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="7">
+        <v>3389726.43</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>827867</v>
+      </c>
+      <c r="F22" s="7">
+        <v>4.0945301962754899</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0.96650000000000003</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.75929999999999997</v>
+      </c>
+      <c r="J22" s="8">
+        <v>5.7254365737491701E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="7">
+        <v>36708903</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2093975</v>
+      </c>
+      <c r="E23" s="9">
+        <v>267919</v>
+      </c>
+      <c r="F23" s="7">
+        <v>137.01492988552499</v>
+      </c>
+      <c r="G23" s="7">
+        <v>7.8157017606067498</v>
+      </c>
+      <c r="H23" s="8">
+        <v>0.88629999999999998</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.41880000000000001</v>
+      </c>
+      <c r="J23" s="8">
+        <v>5.57892497359277E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="7">
+        <v>8576617.5199999996</v>
+      </c>
+      <c r="D24" s="7">
+        <v>556730</v>
+      </c>
+      <c r="E24" s="9">
+        <v>580301</v>
+      </c>
+      <c r="F24" s="7">
+        <v>14.7796014826788</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0.95938142446764696</v>
+      </c>
+      <c r="H24" s="8">
+        <v>0.89759999999999995</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.43880000000000002</v>
+      </c>
+      <c r="J24" s="8">
+        <v>4.2145369385887699E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="8">
-        <v>28479181</v>
-      </c>
-      <c r="D11" s="3">
-        <v>95143</v>
-      </c>
-      <c r="E11" s="8">
-        <v>299.33028178636403</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.5232</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.13059999999999999</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.26953112683014002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="8">
-        <v>168732364</v>
-      </c>
-      <c r="D12" s="3">
-        <v>514278</v>
-      </c>
-      <c r="E12" s="8">
-        <v>328.09562921221601</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="G12" s="4">
-        <v>0.70269999999999999</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0.24448255612723099</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="8">
-        <v>29893961</v>
-      </c>
-      <c r="D13" s="3">
-        <v>59301</v>
-      </c>
-      <c r="E13" s="8">
-        <v>504.10551255459399</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0.62250000000000005</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0.18990000000000001</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0.208984671422067</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8">
-        <v>42819075.789999999</v>
-      </c>
-      <c r="D14" s="3">
-        <v>571818</v>
-      </c>
-      <c r="E14" s="8">
-        <v>74.882350310763201</v>
-      </c>
-      <c r="F14" s="4">
-        <v>0.99129999999999996</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.91539999999999999</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0.168938368501866</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8">
-        <v>2490000</v>
-      </c>
-      <c r="D15" s="3">
-        <v>255635</v>
-      </c>
-      <c r="E15" s="8">
-        <v>9.7404502513349094</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0.81330000000000002</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0.38279999999999997</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0.16756312711483201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="8">
-        <v>80700713</v>
-      </c>
-      <c r="D16" s="3">
-        <v>501928</v>
-      </c>
-      <c r="E16" s="8">
-        <v>160.78145271831801</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0.87949999999999995</v>
-      </c>
-      <c r="G16" s="4">
-        <v>0.44669999999999999</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0.15243421367208002</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="8">
-        <v>26230114</v>
-      </c>
-      <c r="D17" s="3">
-        <v>54486</v>
-      </c>
-      <c r="E17" s="8">
-        <v>481.410160408178</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0.497</v>
-      </c>
-      <c r="G17" s="4">
-        <v>7.5300000000000006E-2</v>
-      </c>
-      <c r="H17" s="4">
-        <v>0.148129794809676</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3">
-        <v>80685</v>
-      </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0.4793</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0.15920000000000001</v>
-      </c>
-      <c r="H18" s="4">
-        <v>0.123628927309909</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3">
-        <v>12557</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0.2145</v>
-      </c>
-      <c r="G19" s="4">
-        <v>6.3399999999999998E-2</v>
-      </c>
-      <c r="H19" s="4">
-        <v>8.7839452098431095E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="8">
-        <v>1349794.92</v>
-      </c>
-      <c r="D20" s="3">
-        <v>438048</v>
-      </c>
-      <c r="E20" s="8">
-        <v>3.0813858755204899</v>
-      </c>
-      <c r="F20" s="4">
-        <v>0.81969999999999998</v>
-      </c>
-      <c r="G20" s="4">
-        <v>0.49370000000000003</v>
-      </c>
-      <c r="H20" s="4">
-        <v>6.4476952297465098E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="8">
-        <v>43923508</v>
-      </c>
-      <c r="D21" s="3">
-        <v>386365</v>
-      </c>
-      <c r="E21" s="8">
-        <v>113.683972409509</v>
-      </c>
-      <c r="F21" s="4">
-        <v>0.83650000000000002</v>
-      </c>
-      <c r="G21" s="4">
-        <v>0.26429999999999998</v>
-      </c>
-      <c r="H21" s="4">
-        <v>6.3608246088543194E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8">
-        <v>3389726.43</v>
-      </c>
-      <c r="D22" s="3">
-        <v>818406</v>
-      </c>
-      <c r="E22" s="8">
-        <v>4.1418640992368099</v>
-      </c>
-      <c r="F22" s="4">
-        <v>0.95550000000000002</v>
-      </c>
-      <c r="G22" s="4">
-        <v>0.78649999999999998</v>
-      </c>
-      <c r="H22" s="4">
-        <v>5.7773281232053497E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="8">
-        <v>36708903</v>
-      </c>
-      <c r="D23" s="3">
-        <v>255768</v>
-      </c>
-      <c r="E23" s="8">
-        <v>143.52422116918501</v>
-      </c>
-      <c r="F23" s="4">
-        <v>0.8528</v>
-      </c>
-      <c r="G23" s="4">
-        <v>0.54330000000000001</v>
-      </c>
-      <c r="H23" s="4">
-        <v>5.3235744893810007E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="8">
-        <v>8576617.5199999996</v>
-      </c>
-      <c r="D24" s="3">
-        <v>570118</v>
-      </c>
-      <c r="E24" s="8">
-        <v>15.0435831178809</v>
-      </c>
-      <c r="F24" s="4">
-        <v>0.88180000000000003</v>
-      </c>
-      <c r="G24" s="4">
-        <v>0.49259999999999998</v>
-      </c>
-      <c r="H24" s="4">
-        <v>4.2468401278331902E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="8">
+      <c r="B25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="7">
         <v>12482869</v>
       </c>
-      <c r="D25" s="3">
-        <v>69186</v>
-      </c>
-      <c r="E25" s="8">
-        <v>180.42478247044201</v>
-      </c>
-      <c r="F25" s="4">
-        <v>0.47970000000000002</v>
-      </c>
-      <c r="G25" s="4">
-        <v>0.1212</v>
-      </c>
-      <c r="H25" s="4">
-        <v>2.9254473448385498E-2</v>
+      <c r="D25" s="7">
+        <v>1471778</v>
+      </c>
+      <c r="E25" s="9">
+        <v>74119</v>
+      </c>
+      <c r="F25" s="7">
+        <v>168.41658684008101</v>
+      </c>
+      <c r="G25" s="7">
+        <v>19.856959753909301</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0.51390000000000002</v>
+      </c>
+      <c r="I25" s="8">
+        <v>9.4100000000000003E-2</v>
+      </c>
+      <c r="J25" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H25" xr:uid="{368E7D20-9635-4E47-860B-FD9183803BB6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H25">
-      <sortCondition descending="1" ref="H1:H25"/>
+  <autoFilter ref="A1:J25" xr:uid="{368E7D20-9635-4E47-860B-FD9183803BB6}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J25">
+      <sortCondition descending="1" ref="J1:J25"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>